<commit_message>
replaces saudi and qatar files with updated files, replaces spaces in file names with underscores
</commit_message>
<xml_diff>
--- a/donor/SaudiArabia_TUFFDonorDataset_Level1_v1.0.xlsx
+++ b/donor/SaudiArabia_TUFFDonorDataset_Level1_v1.0.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17680" windowHeight="16100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17685" windowHeight="16095"/>
   </bookViews>
   <sheets>
     <sheet name="KSATUFF_1.0version" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4645" uniqueCount="1340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4621" uniqueCount="1334">
   <si>
     <t>project_id</t>
   </si>
@@ -3190,24 +3195,6 @@
   </si>
   <si>
     <t xml:space="preserve">Eng. Yousef bin Ibrahim Al-Bassam, CEO (3PL); Salah Al-Deen Mizwar, Moroccan Minister of Economy and Finance </t>
-  </si>
-  <si>
-    <t>Saudi Development Fund endorsing 100 Million Dollar Soft Loan to convert El Shabab &amp; Damietta power stations to the combined cycle technology</t>
-  </si>
-  <si>
-    <t>In 2014, the Saudi Fund for Development gave a 100 million USD soft loan to fund two power plant construction projects in Egypt. The project is cofinanced by the European Bank for Reconstruction and Development (EBRD), European Investment Bank (EIB), and Islamic Development Bank. The Egyptian Electric Holding Company (EEHC) will finance and oversee the conversion project, which is to have a total cost of nearly 4 billion EGP. The project includes Damietta West 500 MW Conversion Project and El Shabab 1000 MW Conversion Project.</t>
-  </si>
-  <si>
-    <t>https://global.factiva.com/aa/?ref=AMCEPN0020131230e9c30004q&amp;pp=1&amp;fcpil=en&amp;napc=S&amp;sa_from=, Media Report, including Wikileaks; http://www.ebrd.com/pages/workingwithus/procurement/notices/project/130926a.shtml, Government Source (Donor/Recipient); http://www.africa-energy.com/egypt-eib-approves-loan-for-el-shabab-power-station, Other Official Source (non-Donor, non-Recipient)</t>
-  </si>
-  <si>
-    <t>Egyptian Electric Holding Company</t>
-  </si>
-  <si>
-    <t>https://global.factiva.com/aa/?ref=AMCEPN0020131230e9c30004q&amp;pp=1&amp;fcpil=en&amp;napc=S&amp;sa_from=, Media Report, including Wikileaks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eng. Mohamed Emam, Minister of Electricity &amp; Energy ; Eng. Gaber Al Dessouki, Chairman of EEHC - Egyptian Electricity Holding Co. </t>
   </si>
   <si>
     <t>Saudi Development Fund loans Morocco 90 million SR to build schools</t>
@@ -4046,10 +4033,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4564,7 +4551,7 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4952,26 +4939,26 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5008,8 +4995,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="478">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5493,6 +5480,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -5751,7 +5746,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5759,52 +5754,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN230"/>
+  <dimension ref="A1:BN229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.5" style="2"/>
-    <col min="4" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="2"/>
-    <col min="7" max="7" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.5" style="2"/>
-    <col min="11" max="11" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11.5" style="2"/>
-    <col min="15" max="15" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="11.5" style="2"/>
-    <col min="19" max="19" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="2"/>
-    <col min="21" max="21" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5" style="2"/>
-    <col min="23" max="23" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="2"/>
-    <col min="25" max="25" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5" style="2"/>
-    <col min="27" max="27" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5" style="2"/>
-    <col min="29" max="29" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5" style="2"/>
+    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="5" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.42578125" style="2"/>
+    <col min="15" max="15" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="11.42578125" style="2"/>
+    <col min="19" max="19" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="2"/>
+    <col min="21" max="21" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="2"/>
+    <col min="23" max="23" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" style="2"/>
+    <col min="25" max="25" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="2"/>
+    <col min="27" max="27" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="2"/>
+    <col min="29" max="29" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="2"/>
     <col min="31" max="31" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.5" style="2"/>
-    <col min="33" max="34" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.33203125" style="2" customWidth="1"/>
-    <col min="36" max="41" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.5" style="2"/>
-    <col min="43" max="44" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.5" style="2"/>
-    <col min="48" max="53" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.5" style="2"/>
-    <col min="55" max="58" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="11.5" style="2"/>
-    <col min="62" max="62" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="11.5" style="2"/>
+    <col min="32" max="32" width="11.42578125" style="2"/>
+    <col min="33" max="34" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" style="2" customWidth="1"/>
+    <col min="36" max="41" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" style="2"/>
+    <col min="43" max="44" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.42578125" style="2"/>
+    <col min="48" max="53" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.42578125" style="2"/>
+    <col min="55" max="58" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.42578125" style="2"/>
+    <col min="62" max="62" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" s="3" customFormat="1">
@@ -5995,16 +5990,16 @@
         <v>61</v>
       </c>
       <c r="BK1" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="BN1" s="3" t="s">
         <v>1333</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>1338</v>
-      </c>
-      <c r="BN1" s="3" t="s">
-        <v>1339</v>
       </c>
     </row>
     <row r="2" spans="1:66">
@@ -6015,7 +6010,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="D2" s="2">
         <v>2011</v>
@@ -6024,7 +6019,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="G2" s="2">
         <v>700</v>
@@ -6045,7 +6040,7 @@
         <v>676</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -6129,7 +6124,7 @@
         <v>41915.702349537038</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="BJ2" s="2">
         <v>1</v>
@@ -6153,7 +6148,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="D3" s="2">
         <v>2010</v>
@@ -6162,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="G3" s="2">
         <v>310</v>
@@ -6171,7 +6166,7 @@
         <v>365</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>107</v>
@@ -6186,7 +6181,7 @@
         <v>366</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="O3" s="2">
         <v>6</v>
@@ -6195,10 +6190,10 @@
         <v>145</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="S3" s="2">
         <v>5</v>
@@ -6228,7 +6223,7 @@
         <v>1</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="AO3" s="2">
         <v>1</v>
@@ -6468,7 +6463,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>260</v>
@@ -6717,7 +6712,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="D7" s="2">
         <v>2011</v>
@@ -6726,7 +6721,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="G7" s="2">
         <v>700</v>
@@ -6747,7 +6742,7 @@
         <v>164</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="O7" s="2">
         <v>3</v>
@@ -6786,7 +6781,7 @@
         <v>1</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="AO7" s="2">
         <v>1</v>
@@ -6831,10 +6826,10 @@
         <v>41810.408136574071</v>
       </c>
       <c r="BH7" s="2" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="BI7" s="2" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="BJ7" s="2">
         <v>1</v>
@@ -6996,7 +6991,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="D9" s="2">
         <v>2011</v>
@@ -7005,7 +7000,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="G9" s="2">
         <v>998</v>
@@ -7026,7 +7021,7 @@
         <v>164</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="O9" s="2">
         <v>2</v>
@@ -7065,7 +7060,7 @@
         <v>1</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="AK9" s="5">
         <v>40725</v>
@@ -7137,7 +7132,7 @@
         <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="D10" s="2">
         <v>2013</v>
@@ -7146,7 +7141,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
       <c r="G10" s="2">
         <v>140</v>
@@ -7167,7 +7162,7 @@
         <v>133</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
       <c r="O10" s="2">
         <v>2</v>
@@ -7206,7 +7201,7 @@
         <v>1</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="AO10" s="2">
         <v>1</v>
@@ -7251,10 +7246,10 @@
         <v>41918.474039351851</v>
       </c>
       <c r="BH10" s="2" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
       <c r="BI10" s="2" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="BJ10" s="2">
         <v>1</v>
@@ -7557,7 +7552,7 @@
         <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1241</v>
+        <v>1235</v>
       </c>
       <c r="D13" s="2">
         <v>2012</v>
@@ -7566,7 +7561,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>1242</v>
+        <v>1236</v>
       </c>
       <c r="G13" s="2">
         <v>700</v>
@@ -7587,7 +7582,7 @@
         <v>133</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="O13" s="2">
         <v>4</v>
@@ -7635,7 +7630,7 @@
         <v>1</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>1244</v>
+        <v>1238</v>
       </c>
       <c r="AO13" s="2">
         <v>1</v>
@@ -7680,7 +7675,7 @@
         <v>41887.379895833335</v>
       </c>
       <c r="BH13" s="2" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="BJ13" s="2">
         <v>1</v>
@@ -8652,7 +8647,7 @@
         <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="D21" s="2">
         <v>2011</v>
@@ -8661,7 +8656,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="G21" s="2">
         <v>520</v>
@@ -8682,13 +8677,13 @@
         <v>355</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="O21" s="2">
         <v>3</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="V21" s="2" t="s">
         <v>69</v>
@@ -8757,10 +8752,10 @@
         <v>41919.610752314817</v>
       </c>
       <c r="BH21" s="2" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="BI21" s="2" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="BJ21" s="2">
         <v>1</v>
@@ -9699,7 +9694,7 @@
         <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1224</v>
+        <v>1218</v>
       </c>
       <c r="D29" s="2">
         <v>2012</v>
@@ -9708,7 +9703,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>1225</v>
+        <v>1219</v>
       </c>
       <c r="G29" s="2">
         <v>700</v>
@@ -9729,13 +9724,13 @@
         <v>133</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>1226</v>
+        <v>1220</v>
       </c>
       <c r="O29" s="2">
         <v>3</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>1227</v>
+        <v>1221</v>
       </c>
       <c r="V29" s="2" t="s">
         <v>69</v>
@@ -9804,7 +9799,7 @@
         <v>42221.334733796299</v>
       </c>
       <c r="BH29" s="2" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="BJ29" s="2">
         <v>1</v>
@@ -10722,7 +10717,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="D37" s="2">
         <v>2013</v>
@@ -10731,7 +10726,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="G37" s="2">
         <v>700</v>
@@ -10752,7 +10747,7 @@
         <v>133</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>1199</v>
+        <v>1193</v>
       </c>
       <c r="O37" s="2">
         <v>1</v>
@@ -10782,7 +10777,7 @@
         <v>1</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>1199</v>
+        <v>1193</v>
       </c>
       <c r="AO37" s="2">
         <v>1</v>
@@ -10827,10 +10822,10 @@
         <v>41914.621631944443</v>
       </c>
       <c r="BH37" s="2" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="BI37" s="2" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="BJ37" s="2">
         <v>1</v>
@@ -10854,7 +10849,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1196</v>
+        <v>1190</v>
       </c>
       <c r="D38" s="2">
         <v>2013</v>
@@ -10863,7 +10858,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>1197</v>
+        <v>1191</v>
       </c>
       <c r="G38" s="2">
         <v>700</v>
@@ -10884,7 +10879,7 @@
         <v>133</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>1198</v>
+        <v>1192</v>
       </c>
       <c r="O38" s="2">
         <v>4</v>
@@ -10914,7 +10909,7 @@
         <v>1</v>
       </c>
       <c r="AD38" s="2" t="s">
-        <v>1199</v>
+        <v>1193</v>
       </c>
       <c r="AO38" s="2">
         <v>1</v>
@@ -10962,7 +10957,7 @@
         <v>1012</v>
       </c>
       <c r="BI38" s="2" t="s">
-        <v>1200</v>
+        <v>1194</v>
       </c>
       <c r="BJ38" s="2">
         <v>1</v>
@@ -10986,7 +10981,7 @@
         <v>62</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1201</v>
+        <v>1195</v>
       </c>
       <c r="D39" s="2">
         <v>2012</v>
@@ -10995,7 +10990,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>1202</v>
+        <v>1196</v>
       </c>
       <c r="G39" s="2">
         <v>120</v>
@@ -11016,7 +11011,7 @@
         <v>133</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>1203</v>
+        <v>1197</v>
       </c>
       <c r="O39" s="2">
         <v>2</v>
@@ -11091,10 +11086,10 @@
         <v>41914.61755787037</v>
       </c>
       <c r="BH39" s="2" t="s">
-        <v>1204</v>
+        <v>1198</v>
       </c>
       <c r="BI39" s="2" t="s">
-        <v>1205</v>
+        <v>1199</v>
       </c>
       <c r="BJ39" s="2">
         <v>1</v>
@@ -13095,7 +13090,7 @@
         <v>62</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
       <c r="D55" s="2">
         <v>2010</v>
@@ -13104,7 +13099,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="G55" s="2">
         <v>700</v>
@@ -13125,7 +13120,7 @@
         <v>164</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="O55" s="2">
         <v>3</v>
@@ -13155,7 +13150,7 @@
         <v>1</v>
       </c>
       <c r="AD55" s="2" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="AO55" s="2">
         <v>1</v>
@@ -13200,10 +13195,10 @@
         <v>41810.429571759261</v>
       </c>
       <c r="BH55" s="2" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
       <c r="BI55" s="2" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="BJ55" s="2">
         <v>1</v>
@@ -13227,7 +13222,7 @@
         <v>62</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1228</v>
+        <v>1222</v>
       </c>
       <c r="D56" s="2">
         <v>2011</v>
@@ -13236,7 +13231,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>1229</v>
+        <v>1223</v>
       </c>
       <c r="G56" s="2">
         <v>700</v>
@@ -13257,7 +13252,7 @@
         <v>164</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>1230</v>
+        <v>1224</v>
       </c>
       <c r="O56" s="2">
         <v>2</v>
@@ -13329,7 +13324,7 @@
         <v>41918.555625000001</v>
       </c>
       <c r="BH56" s="2" t="s">
-        <v>1231</v>
+        <v>1225</v>
       </c>
       <c r="BJ56" s="2">
         <v>1</v>
@@ -13353,7 +13348,7 @@
         <v>62</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>1210</v>
+        <v>1204</v>
       </c>
       <c r="D57" s="2">
         <v>2010</v>
@@ -13362,7 +13357,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>1211</v>
+        <v>1205</v>
       </c>
       <c r="G57" s="2">
         <v>700</v>
@@ -13383,7 +13378,7 @@
         <v>164</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>1212</v>
+        <v>1206</v>
       </c>
       <c r="O57" s="2">
         <v>1</v>
@@ -13455,7 +13450,7 @@
         <v>41886.503055555557</v>
       </c>
       <c r="BH57" s="2" t="s">
-        <v>1213</v>
+        <v>1207</v>
       </c>
       <c r="BJ57" s="2">
         <v>1</v>
@@ -13734,7 +13729,7 @@
         <v>62</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>1186</v>
+        <v>1180</v>
       </c>
       <c r="D60" s="2">
         <v>2013</v>
@@ -13743,7 +13738,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>1187</v>
+        <v>1181</v>
       </c>
       <c r="G60" s="2">
         <v>160</v>
@@ -13764,13 +13759,13 @@
         <v>164</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>1188</v>
+        <v>1182</v>
       </c>
       <c r="O60" s="2">
         <v>3</v>
       </c>
       <c r="T60" s="2" t="s">
-        <v>1189</v>
+        <v>1183</v>
       </c>
       <c r="U60" s="2">
         <v>1</v>
@@ -13800,7 +13795,7 @@
         <v>1</v>
       </c>
       <c r="AD60" s="2" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
       <c r="AM60" s="5">
         <v>41410</v>
@@ -13851,7 +13846,7 @@
         <v>325</v>
       </c>
       <c r="BI60" s="2" t="s">
-        <v>1191</v>
+        <v>1185</v>
       </c>
       <c r="BJ60" s="2">
         <v>1</v>
@@ -13875,7 +13870,7 @@
         <v>62</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="D61" s="2">
         <v>2010</v>
@@ -13884,7 +13879,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="G61" s="2">
         <v>700</v>
@@ -13905,7 +13900,7 @@
         <v>164</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="O61" s="2">
         <v>2</v>
@@ -13935,7 +13930,7 @@
         <v>1</v>
       </c>
       <c r="AD61" s="2" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
       <c r="AO61" s="2">
         <v>1</v>
@@ -13980,7 +13975,7 @@
         <v>41915.691736111112</v>
       </c>
       <c r="BI61" s="2" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="BJ61" s="2">
         <v>1</v>
@@ -14268,7 +14263,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
       <c r="D64" s="2">
         <v>2011</v>
@@ -14277,7 +14272,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="G64" s="2">
         <v>520</v>
@@ -14298,7 +14293,7 @@
         <v>164</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="O64" s="2">
         <v>2</v>
@@ -14328,7 +14323,7 @@
         <v>1</v>
       </c>
       <c r="AD64" s="2" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="AO64" s="2">
         <v>1</v>
@@ -14373,7 +14368,7 @@
         <v>41843.764363425929</v>
       </c>
       <c r="BI64" s="2" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="BJ64" s="2">
         <v>1</v>
@@ -15165,7 +15160,7 @@
         <v>62</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="D71" s="2">
         <v>2012</v>
@@ -15174,7 +15169,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="G71" s="2">
         <v>520</v>
@@ -15195,7 +15190,7 @@
         <v>164</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="O71" s="2">
         <v>2</v>
@@ -15225,7 +15220,7 @@
         <v>1</v>
       </c>
       <c r="AD71" s="2" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="AO71" s="2">
         <v>1</v>
@@ -15270,7 +15265,7 @@
         <v>41841.571203703701</v>
       </c>
       <c r="BI71" s="2" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="BJ71" s="2">
         <v>1</v>
@@ -15294,7 +15289,7 @@
         <v>62</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="D72" s="2">
         <v>2012</v>
@@ -15303,7 +15298,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
       <c r="G72" s="2">
         <v>160</v>
@@ -15324,7 +15319,7 @@
         <v>164</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>1234</v>
+        <v>1228</v>
       </c>
       <c r="O72" s="2">
         <v>4</v>
@@ -15396,7 +15391,7 @@
         <v>41841.582800925928</v>
       </c>
       <c r="BI72" s="2" t="s">
-        <v>1235</v>
+        <v>1229</v>
       </c>
       <c r="BJ72" s="2">
         <v>1</v>
@@ -15693,7 +15688,7 @@
         <v>62</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="D75" s="2">
         <v>2011</v>
@@ -15702,7 +15697,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="G75" s="2">
         <v>700</v>
@@ -15723,7 +15718,7 @@
         <v>676</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="O75" s="2">
         <v>1</v>
@@ -16104,7 +16099,7 @@
         <v>62</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>1192</v>
+        <v>1186</v>
       </c>
       <c r="D78" s="2">
         <v>2012</v>
@@ -16113,7 +16108,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>1193</v>
+        <v>1187</v>
       </c>
       <c r="G78" s="2">
         <v>520</v>
@@ -16134,16 +16129,16 @@
         <v>328</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="O78" s="2">
         <v>1</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>1195</v>
+        <v>1189</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>1195</v>
+        <v>1189</v>
       </c>
       <c r="S78" s="2">
         <v>1</v>
@@ -17259,7 +17254,7 @@
         <v>62</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1206</v>
+        <v>1200</v>
       </c>
       <c r="D87" s="2">
         <v>2011</v>
@@ -17268,7 +17263,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>1207</v>
+        <v>1201</v>
       </c>
       <c r="G87" s="2">
         <v>120</v>
@@ -17289,7 +17284,7 @@
         <v>98</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>1208</v>
+        <v>1202</v>
       </c>
       <c r="O87" s="2">
         <v>3</v>
@@ -17364,7 +17359,7 @@
         <v>821</v>
       </c>
       <c r="BI87" s="2" t="s">
-        <v>1209</v>
+        <v>1203</v>
       </c>
       <c r="BJ87" s="2">
         <v>1</v>
@@ -17388,7 +17383,7 @@
         <v>62</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
       <c r="D88" s="2">
         <v>2012</v>
@@ -17397,7 +17392,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="G88" s="2">
         <v>520</v>
@@ -17418,7 +17413,7 @@
         <v>98</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="O88" s="2">
         <v>5</v>
@@ -19080,7 +19075,7 @@
         <v>1</v>
       </c>
       <c r="BK99" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL99" s="2">
         <v>6</v>
@@ -19101,7 +19096,7 @@
         <v>62</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="D100" s="2">
         <v>2010</v>
@@ -19110,7 +19105,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="G100" s="2">
         <v>230</v>
@@ -19131,7 +19126,7 @@
         <v>133</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>1169</v>
+        <v>1163</v>
       </c>
       <c r="O100" s="2">
         <v>6</v>
@@ -19140,7 +19135,7 @@
         <v>145</v>
       </c>
       <c r="Q100" s="2" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="R100" s="2" t="s">
         <v>145</v>
@@ -19149,7 +19144,7 @@
         <v>1</v>
       </c>
       <c r="T100" s="2" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="U100" s="2">
         <v>1</v>
@@ -19179,7 +19174,7 @@
         <v>1</v>
       </c>
       <c r="AD100" s="2" t="s">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="AE100" s="6">
         <v>193000000</v>
@@ -19262,13 +19257,13 @@
         <v>42248.645856481482</v>
       </c>
       <c r="BH100" s="2" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="BJ100" s="2">
         <v>1</v>
       </c>
       <c r="BK100" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL100" s="2">
         <v>4</v>
@@ -19289,7 +19284,7 @@
         <v>62</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1182</v>
+        <v>1176</v>
       </c>
       <c r="D101" s="2">
         <v>2010</v>
@@ -19298,7 +19293,7 @@
         <v>0</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="G101" s="2">
         <v>230</v>
@@ -19319,7 +19314,7 @@
         <v>366</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>1184</v>
+        <v>1178</v>
       </c>
       <c r="O101" s="2">
         <v>5</v>
@@ -19420,13 +19415,13 @@
         <v>42227.568877314814</v>
       </c>
       <c r="BH101" s="2" t="s">
-        <v>1185</v>
+        <v>1179</v>
       </c>
       <c r="BJ101" s="2">
         <v>1</v>
       </c>
       <c r="BK101" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL101" s="2">
         <v>3</v>
@@ -19447,7 +19442,7 @@
         <v>62</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
       <c r="D102" s="2">
         <v>2010</v>
@@ -19456,7 +19451,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="G102" s="2">
         <v>110</v>
@@ -19477,7 +19472,7 @@
         <v>1047</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="O102" s="2">
         <v>6</v>
@@ -19486,7 +19481,7 @@
         <v>145</v>
       </c>
       <c r="Q102" s="2" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="R102" s="2" t="s">
         <v>145</v>
@@ -19495,7 +19490,7 @@
         <v>1</v>
       </c>
       <c r="T102" s="2" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="U102" s="2">
         <v>1</v>
@@ -19525,7 +19520,7 @@
         <v>1</v>
       </c>
       <c r="AD102" s="2" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
       <c r="AE102" s="6">
         <v>90000000</v>
@@ -19593,13 +19588,13 @@
         <v>42248.642407407409</v>
       </c>
       <c r="BH102" s="2" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="BJ102" s="2">
         <v>1</v>
       </c>
       <c r="BK102" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL102" s="2">
         <v>4</v>
@@ -19939,7 +19934,7 @@
         <v>62</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="D105" s="2">
         <v>2010</v>
@@ -19948,7 +19943,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
       <c r="G105" s="2">
         <v>700</v>
@@ -19969,7 +19964,7 @@
         <v>164</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="O105" s="2">
         <v>1</v>
@@ -19999,7 +19994,7 @@
         <v>1</v>
       </c>
       <c r="AD105" s="2" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="AE105" s="6">
         <v>2000000</v>
@@ -20240,7 +20235,7 @@
         <v>62</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="D107" s="2">
         <v>2010</v>
@@ -20249,7 +20244,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="G107" s="2">
         <v>700</v>
@@ -20270,7 +20265,7 @@
         <v>164</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="O107" s="2">
         <v>5</v>
@@ -20362,10 +20357,10 @@
         <v>41809.668877314813</v>
       </c>
       <c r="BH107" s="2" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="BI107" s="2" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="BJ107" s="2">
         <v>1</v>
@@ -20836,7 +20831,7 @@
         <v>62</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="D111" s="2">
         <v>2010</v>
@@ -20845,7 +20840,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="G111" s="2">
         <v>230</v>
@@ -20866,7 +20861,7 @@
         <v>127</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="O111" s="2">
         <v>7</v>
@@ -20914,7 +20909,7 @@
         <v>1</v>
       </c>
       <c r="AD111" s="2" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="AE111" s="6">
         <v>525000000</v>
@@ -20979,13 +20974,13 @@
         <v>42248.644386574073</v>
       </c>
       <c r="BH111" s="2" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="BJ111" s="2">
         <v>1</v>
       </c>
       <c r="BK111" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL111" s="2">
         <v>7</v>
@@ -21158,7 +21153,7 @@
         <v>1</v>
       </c>
       <c r="BK112" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL112" s="2">
         <v>7</v>
@@ -21620,7 +21615,7 @@
         <v>62</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="D116" s="2">
         <v>2010</v>
@@ -21629,7 +21624,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="G116" s="2">
         <v>140</v>
@@ -21650,7 +21645,7 @@
         <v>98</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="O116" s="2">
         <v>7</v>
@@ -21745,7 +21740,7 @@
         <v>41870.68953703704</v>
       </c>
       <c r="BI116" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="BJ116" s="2">
         <v>1</v>
@@ -22368,7 +22363,7 @@
         <v>62</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>1176</v>
+        <v>1170</v>
       </c>
       <c r="D121" s="2">
         <v>2010</v>
@@ -22377,7 +22372,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>1177</v>
+        <v>1171</v>
       </c>
       <c r="G121" s="2">
         <v>240</v>
@@ -22398,7 +22393,7 @@
         <v>98</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
       <c r="O121" s="2">
         <v>3</v>
@@ -22407,7 +22402,7 @@
         <v>145</v>
       </c>
       <c r="Q121" s="2" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="R121" s="2" t="s">
         <v>145</v>
@@ -22416,7 +22411,7 @@
         <v>1</v>
       </c>
       <c r="T121" s="2" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="U121" s="2">
         <v>2</v>
@@ -22446,7 +22441,7 @@
         <v>1</v>
       </c>
       <c r="AD121" s="2" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
       <c r="AE121" s="6">
         <v>23000000</v>
@@ -22511,7 +22506,7 @@
         <v>42223.390486111108</v>
       </c>
       <c r="BI121" s="2" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
       <c r="BJ121" s="2">
         <v>1</v>
@@ -22535,7 +22530,7 @@
         <v>62</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>1173</v>
+        <v>1167</v>
       </c>
       <c r="D122" s="2">
         <v>2010</v>
@@ -22544,7 +22539,7 @@
         <v>0</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>1174</v>
+        <v>1168</v>
       </c>
       <c r="G122" s="2">
         <v>430</v>
@@ -22565,7 +22560,7 @@
         <v>98</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>1175</v>
+        <v>1169</v>
       </c>
       <c r="O122" s="2">
         <v>1</v>
@@ -22604,7 +22599,7 @@
         <v>1</v>
       </c>
       <c r="AD122" s="2" t="s">
-        <v>1175</v>
+        <v>1169</v>
       </c>
       <c r="AE122" s="6">
         <v>90000000</v>
@@ -22988,7 +22983,7 @@
         <v>1</v>
       </c>
       <c r="BK124" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL124" s="2">
         <v>5</v>
@@ -23009,7 +23004,7 @@
         <v>62</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="D125" s="2">
         <v>2011</v>
@@ -23018,7 +23013,7 @@
         <v>0</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
       <c r="G125" s="2">
         <v>210</v>
@@ -23039,7 +23034,7 @@
         <v>538</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
       <c r="O125" s="2">
         <v>10</v>
@@ -23048,7 +23043,7 @@
         <v>145</v>
       </c>
       <c r="Q125" s="2" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="R125" s="2" t="s">
         <v>361</v>
@@ -23081,7 +23076,7 @@
         <v>1</v>
       </c>
       <c r="AD125" s="2" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
       <c r="AE125" s="6">
         <v>200000000</v>
@@ -23149,16 +23144,16 @@
         <v>42248.542361111111</v>
       </c>
       <c r="BH125" s="2" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="BI125" s="2" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
       <c r="BJ125" s="2">
         <v>1</v>
       </c>
       <c r="BK125" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL125" s="2">
         <v>7</v>
@@ -23179,7 +23174,7 @@
         <v>62</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="D126" s="2">
         <v>2011</v>
@@ -23188,7 +23183,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="G126" s="2">
         <v>230</v>
@@ -23209,7 +23204,7 @@
         <v>88</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="O126" s="2">
         <v>10</v>
@@ -23218,7 +23213,7 @@
         <v>145</v>
       </c>
       <c r="Q126" s="2" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="R126" s="2" t="s">
         <v>145</v>
@@ -23251,7 +23246,7 @@
         <v>1</v>
       </c>
       <c r="AD126" s="2" t="s">
-        <v>1158</v>
+        <v>1152</v>
       </c>
       <c r="AE126" s="6">
         <v>187500000</v>
@@ -23319,16 +23314,16 @@
         <v>42248.538263888891</v>
       </c>
       <c r="BH126" s="2" t="s">
-        <v>1159</v>
+        <v>1153</v>
       </c>
       <c r="BI126" s="2" t="s">
-        <v>1160</v>
+        <v>1154</v>
       </c>
       <c r="BJ126" s="2">
         <v>1</v>
       </c>
       <c r="BK126" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL126" s="2">
         <v>7</v>
@@ -24121,7 +24116,7 @@
         <v>62</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="D132" s="2">
         <v>2011</v>
@@ -24130,7 +24125,7 @@
         <v>0</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="G132" s="2">
         <v>520</v>
@@ -24151,7 +24146,7 @@
         <v>88</v>
       </c>
       <c r="N132" s="2" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="O132" s="2">
         <v>3</v>
@@ -24184,7 +24179,7 @@
         <v>1</v>
       </c>
       <c r="AD132" s="2" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="AE132" s="6">
         <v>1700000</v>
@@ -24249,7 +24244,7 @@
         <v>42244.50986111111</v>
       </c>
       <c r="BI132" s="2" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
       <c r="BJ132" s="2">
         <v>1</v>
@@ -24428,7 +24423,7 @@
         <v>1</v>
       </c>
       <c r="BK133" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL133" s="2">
         <v>5</v>
@@ -25349,7 +25344,7 @@
         <v>1</v>
       </c>
       <c r="BK139" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL139" s="2">
         <v>7</v>
@@ -25370,7 +25365,7 @@
         <v>62</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
       <c r="D140" s="2">
         <v>2011</v>
@@ -25379,7 +25374,7 @@
         <v>0</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
       <c r="G140" s="2">
         <v>110</v>
@@ -25400,7 +25395,7 @@
         <v>164</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="O140" s="2">
         <v>3</v>
@@ -25412,7 +25407,7 @@
         <v>192</v>
       </c>
       <c r="R140" s="2" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="S140" s="2">
         <v>2</v>
@@ -25442,7 +25437,7 @@
         <v>1</v>
       </c>
       <c r="AD140" s="2" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="AE140" s="6">
         <v>12500000</v>
@@ -25507,10 +25502,10 @@
         <v>41843.672094907408</v>
       </c>
       <c r="BH140" s="2" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="BI140" s="2" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="BJ140" s="2">
         <v>1</v>
@@ -25683,7 +25678,7 @@
         <v>62</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="D142" s="2">
         <v>2011</v>
@@ -25692,7 +25687,7 @@
         <v>0</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="G142" s="2">
         <v>160</v>
@@ -25713,7 +25708,7 @@
         <v>164</v>
       </c>
       <c r="N142" s="2" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="O142" s="2">
         <v>1</v>
@@ -25752,7 +25747,7 @@
         <v>1</v>
       </c>
       <c r="AD142" s="2" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="AE142" s="6">
         <v>56000000</v>
@@ -25817,7 +25812,7 @@
         <v>41843.681006944447</v>
       </c>
       <c r="BI142" s="2" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="BJ142" s="2">
         <v>1</v>
@@ -27287,7 +27282,7 @@
         <v>1</v>
       </c>
       <c r="BK151" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL151" s="2">
         <v>7</v>
@@ -27487,7 +27482,7 @@
         <v>230</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J153" s="2" t="s">
         <v>87</v>
@@ -27782,7 +27777,7 @@
         <v>1</v>
       </c>
       <c r="BK154" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL154" s="2">
         <v>5</v>
@@ -27970,7 +27965,7 @@
         <v>1</v>
       </c>
       <c r="BK155" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL155" s="2">
         <v>8</v>
@@ -28146,7 +28141,7 @@
         <v>1</v>
       </c>
       <c r="BK156" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL156" s="2">
         <v>6</v>
@@ -28313,7 +28308,7 @@
         <v>1</v>
       </c>
       <c r="BK157" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL157" s="2">
         <v>6</v>
@@ -28349,7 +28344,7 @@
         <v>230</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J158" s="2" t="s">
         <v>151</v>
@@ -28787,7 +28782,7 @@
         <v>1</v>
       </c>
       <c r="BK160" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL160" s="2">
         <v>6</v>
@@ -28966,7 +28961,7 @@
         <v>62</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>1161</v>
+        <v>1155</v>
       </c>
       <c r="D162" s="2">
         <v>2012</v>
@@ -28975,7 +28970,7 @@
         <v>0</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G162" s="2">
         <v>240</v>
@@ -28996,7 +28991,7 @@
         <v>133</v>
       </c>
       <c r="N162" s="2" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="O162" s="2">
         <v>2</v>
@@ -29011,7 +29006,7 @@
         <v>1</v>
       </c>
       <c r="T162" s="2" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="U162" s="2">
         <v>1</v>
@@ -29041,7 +29036,7 @@
         <v>1</v>
       </c>
       <c r="AD162" s="2" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="AE162" s="6">
         <v>10000000</v>
@@ -29109,7 +29104,7 @@
         <v>41918.475682870368</v>
       </c>
       <c r="BI162" s="2" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="BJ162" s="2">
         <v>1</v>
@@ -29747,7 +29742,7 @@
         <v>1</v>
       </c>
       <c r="BK166" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL166" s="2">
         <v>9</v>
@@ -29768,7 +29763,7 @@
         <v>62</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="D167" s="2">
         <v>2012</v>
@@ -29777,7 +29772,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="G167" s="2">
         <v>430</v>
@@ -29798,7 +29793,7 @@
         <v>1047</v>
       </c>
       <c r="N167" s="2" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="O167" s="2">
         <v>15</v>
@@ -29834,7 +29829,7 @@
         <v>1</v>
       </c>
       <c r="AD167" s="2" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="AE167" s="6">
         <v>1250000000</v>
@@ -29899,7 +29894,7 @@
         <v>42247.56958333333</v>
       </c>
       <c r="BI167" s="2" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="BJ167" s="2">
         <v>1</v>
@@ -30713,7 +30708,7 @@
         <v>62</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="D173" s="2">
         <v>2012</v>
@@ -30722,7 +30717,7 @@
         <v>0</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>1215</v>
+        <v>1209</v>
       </c>
       <c r="G173" s="2">
         <v>140</v>
@@ -30743,7 +30738,7 @@
         <v>676</v>
       </c>
       <c r="N173" s="2" t="s">
-        <v>1216</v>
+        <v>1210</v>
       </c>
       <c r="O173" s="2">
         <v>3</v>
@@ -30752,7 +30747,7 @@
         <v>526</v>
       </c>
       <c r="Q173" s="2" t="s">
-        <v>1217</v>
+        <v>1211</v>
       </c>
       <c r="R173" s="2" t="s">
         <v>526</v>
@@ -30785,7 +30780,7 @@
         <v>1</v>
       </c>
       <c r="AD173" s="2" t="s">
-        <v>1218</v>
+        <v>1212</v>
       </c>
       <c r="AE173" s="6">
         <v>15000000</v>
@@ -30853,7 +30848,7 @@
         <v>792</v>
       </c>
       <c r="BI173" s="2" t="s">
-        <v>1219</v>
+        <v>1213</v>
       </c>
       <c r="BJ173" s="2">
         <v>1</v>
@@ -31032,7 +31027,7 @@
         <v>62</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>1220</v>
+        <v>1214</v>
       </c>
       <c r="D175" s="2">
         <v>2012</v>
@@ -31041,7 +31036,7 @@
         <v>0</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="G175" s="2">
         <v>700</v>
@@ -31062,7 +31057,7 @@
         <v>676</v>
       </c>
       <c r="N175" s="2" t="s">
-        <v>1222</v>
+        <v>1216</v>
       </c>
       <c r="O175" s="2">
         <v>1</v>
@@ -31166,7 +31161,7 @@
         <v>41914.542916666665</v>
       </c>
       <c r="BI175" s="2" t="s">
-        <v>1223</v>
+        <v>1217</v>
       </c>
       <c r="BJ175" s="2">
         <v>1</v>
@@ -31345,7 +31340,7 @@
         <v>1</v>
       </c>
       <c r="BK176" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL176" s="2">
         <v>5</v>
@@ -31512,7 +31507,7 @@
         <v>62</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="D178" s="2">
         <v>2012</v>
@@ -31521,7 +31516,7 @@
         <v>0</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="G178" s="2">
         <v>230</v>
@@ -31542,7 +31537,7 @@
         <v>495</v>
       </c>
       <c r="N178" s="2" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="O178" s="2">
         <v>10</v>
@@ -31551,7 +31546,7 @@
         <v>145</v>
       </c>
       <c r="Q178" s="2" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="R178" s="2" t="s">
         <v>145</v>
@@ -31584,7 +31579,7 @@
         <v>1</v>
       </c>
       <c r="AD178" s="2" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="AE178" s="6">
         <v>450000000</v>
@@ -31667,13 +31662,13 @@
         <v>42248.697731481479</v>
       </c>
       <c r="BH178" s="2" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="BJ178" s="2">
         <v>1</v>
       </c>
       <c r="BK178" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL178" s="2">
         <v>7</v>
@@ -31694,7 +31689,7 @@
         <v>62</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="D179" s="2">
         <v>2012</v>
@@ -31703,13 +31698,13 @@
         <v>0</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="G179" s="2">
         <v>230</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J179" s="2" t="s">
         <v>151</v>
@@ -31724,7 +31719,7 @@
         <v>495</v>
       </c>
       <c r="N179" s="2" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
       <c r="O179" s="2">
         <v>8</v>
@@ -31733,7 +31728,7 @@
         <v>145</v>
       </c>
       <c r="Q179" s="2" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="R179" s="2" t="s">
         <v>145</v>
@@ -31766,7 +31761,7 @@
         <v>1</v>
       </c>
       <c r="AD179" s="2" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
       <c r="AE179" s="6">
         <v>318750000</v>
@@ -31849,13 +31844,13 @@
         <v>42248.69667824074</v>
       </c>
       <c r="BH179" s="2" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="BJ179" s="2">
         <v>1</v>
       </c>
       <c r="BK179" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL179" s="2">
         <v>7</v>
@@ -31876,7 +31871,7 @@
         <v>62</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="D180" s="2">
         <v>2012</v>
@@ -31885,7 +31880,7 @@
         <v>0</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="G180" s="2">
         <v>110</v>
@@ -31906,7 +31901,7 @@
         <v>495</v>
       </c>
       <c r="N180" s="2" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="O180" s="2">
         <v>12</v>
@@ -31915,7 +31910,7 @@
         <v>145</v>
       </c>
       <c r="Q180" s="2" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="R180" s="2" t="s">
         <v>145</v>
@@ -31924,7 +31919,7 @@
         <v>1</v>
       </c>
       <c r="T180" s="2" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="U180" s="2">
         <v>1</v>
@@ -31954,7 +31949,7 @@
         <v>1</v>
       </c>
       <c r="AD180" s="2" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="AE180" s="6">
         <v>60000000</v>
@@ -32037,7 +32032,7 @@
         <v>1</v>
       </c>
       <c r="BK180" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL180" s="2">
         <v>7</v>
@@ -32204,7 +32199,7 @@
         <v>62</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="D182" s="2">
         <v>2012</v>
@@ -32213,7 +32208,7 @@
         <v>0</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="G182" s="2">
         <v>120</v>
@@ -32234,7 +32229,7 @@
         <v>98</v>
       </c>
       <c r="N182" s="2" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="O182" s="2">
         <v>2</v>
@@ -32273,7 +32268,7 @@
         <v>1</v>
       </c>
       <c r="AD182" s="2" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="AE182" s="6">
         <v>6000000</v>
@@ -32338,7 +32333,7 @@
         <v>41871.471770833334</v>
       </c>
       <c r="BI182" s="2" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="BJ182" s="2">
         <v>1</v>
@@ -32362,7 +32357,7 @@
         <v>62</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="D183" s="2">
         <v>2012</v>
@@ -32371,7 +32366,7 @@
         <v>0</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="G183" s="2">
         <v>230</v>
@@ -32392,7 +32387,7 @@
         <v>98</v>
       </c>
       <c r="N183" s="2" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="O183" s="2">
         <v>4</v>
@@ -32431,7 +32426,7 @@
         <v>1</v>
       </c>
       <c r="AD183" s="2" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="AE183" s="6">
         <v>270000000</v>
@@ -32690,7 +32685,7 @@
         <v>230</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J185" s="2" t="s">
         <v>66</v>
@@ -32982,7 +32977,7 @@
         <v>62</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="D187" s="2">
         <v>2012</v>
@@ -32991,7 +32986,7 @@
         <v>0</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="G187" s="2">
         <v>430</v>
@@ -33012,7 +33007,7 @@
         <v>98</v>
       </c>
       <c r="N187" s="2" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="O187" s="2">
         <v>4</v>
@@ -33042,7 +33037,7 @@
         <v>1</v>
       </c>
       <c r="AD187" s="2" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="AE187" s="6">
         <v>1750000000</v>
@@ -33110,7 +33105,7 @@
         <v>42244.558715277781</v>
       </c>
       <c r="BI187" s="2" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="BJ187" s="2">
         <v>1</v>
@@ -33149,7 +33144,7 @@
         <v>530</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="J188" s="2" t="s">
         <v>87</v>
@@ -33310,7 +33305,7 @@
         <v>230</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J189" s="2" t="s">
         <v>66</v>
@@ -33462,7 +33457,7 @@
         <v>230</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J190" s="2" t="s">
         <v>66</v>
@@ -34377,7 +34372,7 @@
         <v>1</v>
       </c>
       <c r="BK195" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL195" s="2">
         <v>4</v>
@@ -34386,7 +34381,7 @@
         <v>8</v>
       </c>
       <c r="BN195" s="2">
-        <f t="shared" ref="BN195:BN230" si="11">SUM(BL195+BM195)</f>
+        <f t="shared" ref="BN195:BN229" si="11">SUM(BL195+BM195)</f>
         <v>12</v>
       </c>
     </row>
@@ -35450,7 +35445,7 @@
         <v>62</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="D203" s="2">
         <v>2013</v>
@@ -35459,7 +35454,7 @@
         <v>0</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="G203" s="2">
         <v>210</v>
@@ -35480,7 +35475,7 @@
         <v>380</v>
       </c>
       <c r="N203" s="2" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="O203" s="2">
         <v>5</v>
@@ -35489,7 +35484,7 @@
         <v>145</v>
       </c>
       <c r="Q203" s="2" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="R203" s="2" t="s">
         <v>145</v>
@@ -35498,7 +35493,7 @@
         <v>1</v>
       </c>
       <c r="T203" s="2" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="U203" s="2">
         <v>1</v>
@@ -35528,7 +35523,7 @@
         <v>1</v>
       </c>
       <c r="AD203" s="2" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="AE203" s="6">
         <v>56250000</v>
@@ -35602,16 +35597,16 @@
         <v>42248.690706018519</v>
       </c>
       <c r="BH203" s="2" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="BI203" s="2" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="BJ203" s="2">
         <v>1</v>
       </c>
       <c r="BK203" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL203" s="2">
         <v>5</v>
@@ -35775,7 +35770,7 @@
         <v>1</v>
       </c>
       <c r="BK204" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL204" s="2">
         <v>3</v>
@@ -36249,7 +36244,7 @@
         <v>1</v>
       </c>
       <c r="BK207" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL207" s="2">
         <v>6</v>
@@ -36744,7 +36739,7 @@
         <v>62</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="D211" s="2">
         <v>2013</v>
@@ -36753,7 +36748,7 @@
         <v>1</v>
       </c>
       <c r="F211" s="2" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="G211" s="2">
         <v>160</v>
@@ -36774,7 +36769,7 @@
         <v>164</v>
       </c>
       <c r="N211" s="2" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="O211" s="2">
         <v>1</v>
@@ -36813,7 +36808,7 @@
         <v>1</v>
       </c>
       <c r="AD211" s="2" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="AE211" s="6">
         <v>100000000</v>
@@ -36878,7 +36873,7 @@
         <v>41886.598703703705</v>
       </c>
       <c r="BI211" s="2" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="BJ211" s="2">
         <v>1</v>
@@ -36917,7 +36912,7 @@
         <v>230</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J212" s="2" t="s">
         <v>66</v>
@@ -37838,7 +37833,7 @@
         <v>62</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="D218" s="2">
         <v>2013</v>
@@ -37847,7 +37842,7 @@
         <v>0</v>
       </c>
       <c r="F218" s="2" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="G218" s="2">
         <v>430</v>
@@ -37868,7 +37863,7 @@
         <v>328</v>
       </c>
       <c r="N218" s="2" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="O218" s="2">
         <v>2</v>
@@ -38300,7 +38295,7 @@
         <v>62</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>1236</v>
+        <v>1230</v>
       </c>
       <c r="D221" s="2">
         <v>2013</v>
@@ -38309,7 +38304,7 @@
         <v>0</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>1237</v>
+        <v>1231</v>
       </c>
       <c r="G221" s="2">
         <v>700</v>
@@ -38330,7 +38325,7 @@
         <v>127</v>
       </c>
       <c r="N221" s="2" t="s">
-        <v>1238</v>
+        <v>1232</v>
       </c>
       <c r="O221" s="2">
         <v>4</v>
@@ -38363,7 +38358,7 @@
         <v>1</v>
       </c>
       <c r="AD221" s="2" t="s">
-        <v>1239</v>
+        <v>1233</v>
       </c>
       <c r="AE221" s="6">
         <v>7901250</v>
@@ -38428,7 +38423,7 @@
         <v>41884.542511574073</v>
       </c>
       <c r="BI221" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="BJ221" s="2">
         <v>1</v>
@@ -38539,11 +38534,11 @@
         <v>1</v>
       </c>
       <c r="AI222" s="7">
-        <f t="shared" ref="AI222:AI253" si="12">AJ222*AG222</f>
+        <f t="shared" ref="AI222:AI229" si="12">AJ222*AG222</f>
         <v>196000</v>
       </c>
       <c r="AJ222" s="7">
-        <f t="shared" ref="AJ222:AJ230" si="13">AE222*AH222</f>
+        <f t="shared" ref="AJ222:AJ229" si="13">AE222*AH222</f>
         <v>200000</v>
       </c>
       <c r="AO222" s="2">
@@ -38765,7 +38760,7 @@
         <v>1</v>
       </c>
       <c r="BK223" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL223" s="2">
         <v>6</v>
@@ -38786,7 +38781,7 @@
         <v>62</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="D224" s="2">
         <v>2013</v>
@@ -38795,7 +38790,7 @@
         <v>0</v>
       </c>
       <c r="F224" s="2" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="G224" s="2">
         <v>160</v>
@@ -38816,7 +38811,7 @@
         <v>495</v>
       </c>
       <c r="N224" s="2" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="O224" s="2">
         <v>5</v>
@@ -38825,7 +38820,7 @@
         <v>145</v>
       </c>
       <c r="Q224" s="2" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="R224" s="2" t="s">
         <v>145</v>
@@ -38858,7 +38853,7 @@
         <v>1</v>
       </c>
       <c r="AD224" s="2" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="AE224" s="6">
         <v>562500000</v>
@@ -38941,13 +38936,13 @@
         <v>42248.694363425922</v>
       </c>
       <c r="BH224" s="2" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="BJ224" s="2">
         <v>1</v>
       </c>
       <c r="BK224" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="BL224" s="2">
         <v>5</v>
@@ -38968,7 +38963,7 @@
         <v>62</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="D225" s="2">
         <v>2013</v>
@@ -38977,7 +38972,7 @@
         <v>0</v>
       </c>
       <c r="F225" s="2" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="G225" s="2">
         <v>120</v>
@@ -38998,7 +38993,7 @@
         <v>98</v>
       </c>
       <c r="N225" s="2" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="O225" s="2">
         <v>14</v>
@@ -39037,7 +39032,7 @@
         <v>1</v>
       </c>
       <c r="AD225" s="2" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="AE225" s="6">
         <v>200000000</v>
@@ -39123,7 +39118,7 @@
         <v>62</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="D226" s="2">
         <v>2013</v>
@@ -39132,7 +39127,7 @@
         <v>0</v>
       </c>
       <c r="F226" s="2" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="G226" s="2">
         <v>210</v>
@@ -39153,7 +39148,7 @@
         <v>98</v>
       </c>
       <c r="N226" s="2" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="O226" s="2">
         <v>6</v>
@@ -39192,7 +39187,7 @@
         <v>1</v>
       </c>
       <c r="AD226" s="2" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="AE226" s="6">
         <v>50000000</v>
@@ -39433,7 +39428,7 @@
         <v>62</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="D228" s="2">
         <v>2013</v>
@@ -39442,13 +39437,13 @@
         <v>0</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="G228" s="2">
         <v>530</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="J228" s="2" t="s">
         <v>151</v>
@@ -39463,7 +39458,7 @@
         <v>98</v>
       </c>
       <c r="N228" s="2" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="O228" s="2">
         <v>1</v>
@@ -39472,7 +39467,7 @@
         <v>145</v>
       </c>
       <c r="Q228" s="2" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="R228" s="2" t="s">
         <v>145</v>
@@ -39481,7 +39476,7 @@
         <v>1</v>
       </c>
       <c r="T228" s="2" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="U228" s="2">
         <v>1</v>
@@ -39511,7 +39506,7 @@
         <v>1</v>
       </c>
       <c r="AD228" s="2" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="AE228" s="6">
         <v>25000000</v>
@@ -39743,176 +39738,6 @@
         <v>7</v>
       </c>
       <c r="BN229" s="2">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="230" spans="1:66">
-      <c r="A230" s="2">
-        <v>32709</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D230" s="2">
-        <v>2014</v>
-      </c>
-      <c r="E230" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F230" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="G230" s="2">
-        <v>230</v>
-      </c>
-      <c r="H230" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J230" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="K230" s="2">
-        <v>11</v>
-      </c>
-      <c r="L230" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="M230" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N230" s="2" t="s">
-        <v>1059</v>
-      </c>
-      <c r="O230" s="2">
-        <v>3</v>
-      </c>
-      <c r="P230" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="R230" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="S230" s="2">
-        <v>1</v>
-      </c>
-      <c r="T230" s="2" t="s">
-        <v>1060</v>
-      </c>
-      <c r="U230" s="2">
-        <v>1</v>
-      </c>
-      <c r="V230" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="W230" s="2">
-        <v>1</v>
-      </c>
-      <c r="X230" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y230" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z230" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA230" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB230" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC230" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD230" s="2" t="s">
-        <v>1061</v>
-      </c>
-      <c r="AE230" s="6">
-        <v>100000000</v>
-      </c>
-      <c r="AF230" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG230" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="AH230" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI230" s="7">
-        <f t="shared" si="12"/>
-        <v>97000000</v>
-      </c>
-      <c r="AJ230" s="7">
-        <f t="shared" si="13"/>
-        <v>100000000</v>
-      </c>
-      <c r="AO230" s="2">
-        <v>1</v>
-      </c>
-      <c r="AP230" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ230" s="2">
-        <v>651</v>
-      </c>
-      <c r="AR230" s="2">
-        <v>142</v>
-      </c>
-      <c r="AS230" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT230" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU230" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV230" s="2">
-        <v>818</v>
-      </c>
-      <c r="AW230" s="2">
-        <v>469</v>
-      </c>
-      <c r="AX230" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AY230" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ230" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="BA230" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BB230" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="BG230" s="4">
-        <v>42244.639513888891</v>
-      </c>
-      <c r="BI230" s="2" t="s">
-        <v>1062</v>
-      </c>
-      <c r="BJ230" s="2">
-        <v>1</v>
-      </c>
-      <c r="BK230" s="2" t="s">
-        <v>1335</v>
-      </c>
-      <c r="BL230" s="2">
-        <v>6</v>
-      </c>
-      <c r="BM230" s="2">
-        <v>7</v>
-      </c>
-      <c r="BN230" s="2">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>

</xml_diff>